<commit_message>
worked on line balance
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofia/PycharmProjects/Mendelson/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\PycharmProjects\Mendelson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE8A8A5-744A-1148-A27F-F5F8FDA24B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C0FF68-5E7D-4364-8557-C4450EB542B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{76B1A70E-36C2-9E4B-B9BC-6E6D070680C3}"/>
+    <workbookView xWindow="2880" yWindow="2090" windowWidth="14400" windowHeight="7370" xr2:uid="{76B1A70E-36C2-9E4B-B9BC-6E6D070680C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>שם מלא</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>שעת_התחלה</t>
+  </si>
+  <si>
+    <t>שעת_סיום</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,6 +175,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -488,20 +494,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA47D2D1-C530-894D-89EF-E9CDCD152A5D}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="6.1640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" style="8" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,8 +526,11 @@
       <c r="F1" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -540,8 +549,11 @@
       <c r="F2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -560,8 +572,11 @@
       <c r="F3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -580,8 +595,11 @@
       <c r="F4">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -600,8 +618,11 @@
       <c r="F5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -620,8 +641,11 @@
       <c r="F6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -640,8 +664,11 @@
       <c r="F7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -660,8 +687,11 @@
       <c r="F8">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -680,29 +710,32 @@
       <c r="F9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="7"/>

</xml_diff>